<commit_message>
implemented getting project details and editing project
</commit_message>
<xml_diff>
--- a/List of tasks.xlsx
+++ b/List of tasks.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saurabhmane/Developer/College dev/Web/Project/Group_9_CS546_A/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F4C272-3580-8D46-86CA-621C0FBB3791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Strory Name</t>
   </si>
@@ -203,25 +223,37 @@
   </si>
   <si>
     <t>Calculating success rate after project completion</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -229,7 +261,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -245,44 +277,43 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -472,32 +503,43 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="64.57"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="str">
+        <f>D1</f>
+        <v>Status</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="21.0" customHeight="1">
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -508,7 +550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -516,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -524,7 +566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -532,7 +574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -540,7 +582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="21.0" customHeight="1">
+    <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -550,24 +592,33 @@
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" ht="22.5" customHeight="1">
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -577,12 +628,15 @@
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" ht="21.75" customHeight="1">
+    <row r="12" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -592,32 +646,44 @@
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" ht="21.75" customHeight="1">
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -627,16 +693,22 @@
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" ht="22.5" customHeight="1">
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -647,7 +719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -655,7 +727,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -663,7 +735,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" ht="19.5" customHeight="1">
+    <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -674,7 +746,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -682,15 +754,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" ht="21.0" customHeight="1">
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
@@ -701,7 +776,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
@@ -709,7 +784,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
@@ -720,7 +795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -728,7 +803,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
@@ -736,7 +811,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -744,7 +819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" ht="21.75" customHeight="1">
+    <row r="30" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
@@ -755,7 +830,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>62</v>
       </c>
@@ -764,6 +839,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>